<commit_message>
Update UI design. (Kaii)
</commit_message>
<xml_diff>
--- a/PCB/04 Dev_Lib/4.2_Design/UI_Admin_v0.1.xlsx
+++ b/PCB/04 Dev_Lib/4.2_Design/UI_Admin_v0.1.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14680" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Admin(1)" sheetId="2" r:id="rId1"/>
-    <sheet name="Admin(2)" sheetId="3" r:id="rId2"/>
+    <sheet name="Admin(2)" sheetId="8" r:id="rId2"/>
     <sheet name="Admin(3)" sheetId="4" r:id="rId3"/>
     <sheet name="Admin(4)" sheetId="5" r:id="rId4"/>
     <sheet name="Admin(5)" sheetId="6" r:id="rId5"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="46">
   <si>
     <t>Courses</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -54,10 +54,6 @@
   </si>
   <si>
     <t>Price</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Catgory</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -113,10 +109,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>User Catagory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Course Price</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -142,10 +134,6 @@
   </si>
   <si>
     <t>Detail Story</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Target Catagory</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -224,6 +212,18 @@
   <si>
     <t>Brief story…
 …</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Target Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1062,7 +1062,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="800"/>
-            <a:t>Disable</a:t>
+            <a:t>Class</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800"/>
         </a:p>
@@ -1230,7 +1230,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="800"/>
-            <a:t>Disable</a:t>
+            <a:t>Class</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800"/>
         </a:p>
@@ -1398,7 +1398,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="800"/>
-            <a:t>Disable</a:t>
+            <a:t>Class</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800"/>
         </a:p>
@@ -1566,7 +1566,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="800"/>
-            <a:t>Disable</a:t>
+            <a:t>Class</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800"/>
         </a:p>
@@ -1734,7 +1734,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="800"/>
-            <a:t>Disable</a:t>
+            <a:t>Class</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800"/>
         </a:p>
@@ -2071,1593 +2071,6 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>152401</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="组 1"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="280416" y="243840"/>
-          <a:ext cx="11131297" cy="5955792"/>
-          <a:chOff x="279399" y="254000"/>
-          <a:chExt cx="11125201" cy="5918200"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="进程 2"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="279400" y="254000"/>
-            <a:ext cx="11125200" cy="664966"/>
-          </a:xfrm>
-          <a:prstGeom prst="flowChartProcess">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="3">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="1400"/>
-              <a:t>Header :</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
-              <a:t> Dashboard (Common)</a:t>
-            </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="进程 3"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="279400" y="5706724"/>
-            <a:ext cx="11125200" cy="465476"/>
-          </a:xfrm>
-          <a:prstGeom prst="flowChartProcess">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="3">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="1600"/>
-              <a:t>Footer : Contact Info. (Common) </a:t>
-            </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1600"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="同侧圆角矩形 4"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="279400" y="1057025"/>
-            <a:ext cx="2133601" cy="398980"/>
-          </a:xfrm>
-          <a:prstGeom prst="round2SameRect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent3"/>
-          </a:lnRef>
-          <a:fillRef idx="2">
-            <a:schemeClr val="accent3"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent3"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Quick Links</a:t>
-            </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="同侧圆角矩形 5"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="279400" y="2835810"/>
-            <a:ext cx="2133601" cy="398980"/>
-          </a:xfrm>
-          <a:prstGeom prst="round2SameRect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent3"/>
-          </a:lnRef>
-          <a:fillRef idx="2">
-            <a:schemeClr val="accent3"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent3"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>XXX Links</a:t>
-            </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="7" name="矩形 6"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="279399" y="1472629"/>
-            <a:ext cx="2133601" cy="1263436"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent3"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent3"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="矩形 7"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="279399" y="3251414"/>
-            <a:ext cx="2133601" cy="2323886"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent3"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent3"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>431800</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="矩形 23"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2730500" y="3162300"/>
-          <a:ext cx="6743700" cy="393700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="28575" cmpd="sng">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:prstDash val="dash"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>241300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>330200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="线形标注 2 (无边框) 24"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9931400" y="2451100"/>
-          <a:ext cx="1981200" cy="546100"/>
-        </a:xfrm>
-        <a:prstGeom prst="callout2">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 18750"/>
-            <a:gd name="adj2" fmla="val -8333"/>
-            <a:gd name="adj3" fmla="val 18750"/>
-            <a:gd name="adj4" fmla="val -16667"/>
-            <a:gd name="adj5" fmla="val 170640"/>
-            <a:gd name="adj6" fmla="val -39211"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:prstDash val="dash"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent4"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent4"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>&lt;1&gt;</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>New data</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> / new DB item</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1231899</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>618066</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="可选流程 26"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4038599" y="4559300"/>
-          <a:ext cx="859367" cy="241300"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartAlternateProcess">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="3">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="0" rIns="0" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="800"/>
-            <a:t>Submit</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1231899</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>507999</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>330200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="矩形 27"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4038599" y="1333500"/>
-          <a:ext cx="2590800" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="3175" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1231899</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>78317</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>507999</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>332317</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="矩形 28"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4038599" y="1792817"/>
-          <a:ext cx="2590800" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="3175" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1231899</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>86785</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>507999</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>340785</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="矩形 32"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4038599" y="3668185"/>
-          <a:ext cx="2590800" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="3175" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1231899</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>507999</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="矩形 33"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4038599" y="4089400"/>
-          <a:ext cx="2590800" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="3175" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1231899</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>80434</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>507999</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>334434</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="38" name="组 37"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="4044695" y="2302426"/>
-          <a:ext cx="2593848" cy="256032"/>
-          <a:chOff x="4038599" y="2290234"/>
-          <a:chExt cx="2590800" cy="254000"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="30" name="矩形 29"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4038599" y="2290234"/>
-            <a:ext cx="2590800" cy="254000"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg1"/>
-          </a:solidFill>
-          <a:ln w="3175" cmpd="sng">
-            <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent5"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
-              <a:t>Please select </a:t>
-            </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="35" name="合并 34"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6400800" y="2349500"/>
-            <a:ext cx="180000" cy="141800"/>
-          </a:xfrm>
-          <a:prstGeom prst="flowChartMerge">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="50000"/>
-              <a:lumOff val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="dk1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1231899</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>82551</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>507999</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>336551</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="39" name="组 38"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="4044695" y="2764283"/>
-          <a:ext cx="2593848" cy="256032"/>
-          <a:chOff x="4038599" y="2749551"/>
-          <a:chExt cx="2590800" cy="254000"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="31" name="矩形 30"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4038599" y="2749551"/>
-            <a:ext cx="2590800" cy="254000"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg1"/>
-          </a:solidFill>
-          <a:ln w="3175" cmpd="sng">
-            <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent5"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
-              <a:t>Please select</a:t>
-            </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="37" name="合并 36"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6400800" y="2806700"/>
-            <a:ext cx="180000" cy="141800"/>
-          </a:xfrm>
-          <a:prstGeom prst="flowChartMerge">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="50000"/>
-              <a:lumOff val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="dk1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1231899</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>64093</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>376768</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="57" name="组 56"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="4044695" y="3258312"/>
-          <a:ext cx="5209626" cy="263992"/>
-          <a:chOff x="6845300" y="3200400"/>
-          <a:chExt cx="5207594" cy="262468"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="43" name="组 42"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="6845300" y="3200400"/>
-            <a:ext cx="1003300" cy="262468"/>
-            <a:chOff x="6845300" y="3200400"/>
-            <a:chExt cx="1003300" cy="262468"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="41" name="矩形 40"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6997699" y="3200400"/>
-              <a:ext cx="850901" cy="262468"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="3175" cmpd="sng">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent5"/>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="lt1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent5"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:r>
-                <a:rPr lang="en-US" altLang="zh-CN" sz="1000"/>
-                <a:t>Company</a:t>
-              </a:r>
-              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="42" name="进程 41"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6845300" y="3251200"/>
-              <a:ext cx="141800" cy="141800"/>
-            </a:xfrm>
-            <a:prstGeom prst="flowChartProcess">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="lt1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="44" name="组 43"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="7962900" y="3200400"/>
-            <a:ext cx="1003300" cy="262468"/>
-            <a:chOff x="6845300" y="3200400"/>
-            <a:chExt cx="1003300" cy="262468"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="45" name="矩形 44"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6997699" y="3200400"/>
-              <a:ext cx="850901" cy="262468"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="3175" cmpd="sng">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent5"/>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="lt1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent5"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:r>
-                <a:rPr lang="en-US" altLang="zh-CN" sz="1000"/>
-                <a:t>Student</a:t>
-              </a:r>
-              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="46" name="进程 45"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6845300" y="3251200"/>
-              <a:ext cx="141800" cy="141800"/>
-            </a:xfrm>
-            <a:prstGeom prst="flowChartProcess">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="lt1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="47" name="组 46"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="8928100" y="3200400"/>
-            <a:ext cx="1003300" cy="262468"/>
-            <a:chOff x="6845300" y="3200400"/>
-            <a:chExt cx="1003300" cy="262468"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="48" name="矩形 47"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6997699" y="3200400"/>
-              <a:ext cx="850901" cy="262468"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="3175" cmpd="sng">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent5"/>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="lt1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent5"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:r>
-                <a:rPr lang="en-US" altLang="zh-CN" sz="1000"/>
-                <a:t>Migrant</a:t>
-              </a:r>
-              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="49" name="进程 48"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6845300" y="3251200"/>
-              <a:ext cx="141800" cy="141800"/>
-            </a:xfrm>
-            <a:prstGeom prst="flowChartProcess">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="lt1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="50" name="组 49"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="9906000" y="3200400"/>
-            <a:ext cx="1003300" cy="262468"/>
-            <a:chOff x="6845300" y="3200400"/>
-            <a:chExt cx="1003300" cy="262468"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="51" name="矩形 50"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6997699" y="3200400"/>
-              <a:ext cx="850901" cy="262468"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="3175" cmpd="sng">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent5"/>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="lt1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent5"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:r>
-                <a:rPr lang="en-US" altLang="zh-CN" sz="1000"/>
-                <a:t>Kiwi</a:t>
-              </a:r>
-              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="52" name="进程 51"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6845300" y="3251200"/>
-              <a:ext cx="141800" cy="141800"/>
-            </a:xfrm>
-            <a:prstGeom prst="flowChartProcess">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="lt1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="56" name="组 55"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="10604500" y="3200400"/>
-            <a:ext cx="1448394" cy="262468"/>
-            <a:chOff x="8877300" y="4114800"/>
-            <a:chExt cx="1448394" cy="262468"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="54" name="矩形 53"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="9029697" y="4114800"/>
-              <a:ext cx="1295997" cy="262468"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="3175" cmpd="sng">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent5"/>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="lt1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent5"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:r>
-                <a:rPr lang="en-US" altLang="zh-CN" sz="1000"/>
-                <a:t>Career</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" altLang="zh-CN" sz="1000" baseline="0"/>
-                <a:t> Changer</a:t>
-              </a:r>
-              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="55" name="进程 54"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="8877300" y="4165600"/>
-              <a:ext cx="141800" cy="141800"/>
-            </a:xfrm>
-            <a:prstGeom prst="flowChartProcess">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="lt1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>1</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -3673,8 +2086,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="280416" y="256032"/>
-          <a:ext cx="11131297" cy="5955792"/>
+          <a:off x="279400" y="254000"/>
+          <a:ext cx="11125201" cy="5918200"/>
           <a:chOff x="279399" y="254000"/>
           <a:chExt cx="11125201" cy="5918200"/>
         </a:xfrm>
@@ -4366,7 +2779,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4093632" y="4601633"/>
+          <a:off x="4038599" y="4584700"/>
           <a:ext cx="452968" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4429,8 +2842,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4044695" y="2302426"/>
-          <a:ext cx="2593848" cy="256032"/>
+          <a:off x="4038599" y="2290234"/>
+          <a:ext cx="2590800" cy="254000"/>
           <a:chOff x="4038599" y="2290234"/>
           <a:chExt cx="2590800" cy="254000"/>
         </a:xfrm>
@@ -4563,8 +2976,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4044695" y="2764283"/>
-          <a:ext cx="2593848" cy="256032"/>
+          <a:off x="4038599" y="2749551"/>
+          <a:ext cx="2590800" cy="254000"/>
           <a:chOff x="4038599" y="2749551"/>
           <a:chExt cx="2590800" cy="254000"/>
         </a:xfrm>
@@ -4697,8 +3110,1847 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4044695" y="3258312"/>
-          <a:ext cx="5209626" cy="263992"/>
+          <a:off x="4038599" y="3238500"/>
+          <a:ext cx="5207594" cy="262468"/>
+          <a:chOff x="6845300" y="3200400"/>
+          <a:chExt cx="5207594" cy="262468"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="23" name="组 22"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="6845300" y="3200400"/>
+            <a:ext cx="1003300" cy="262468"/>
+            <a:chOff x="6845300" y="3200400"/>
+            <a:chExt cx="1003300" cy="262468"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="36" name="矩形 35"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6997699" y="3200400"/>
+              <a:ext cx="850901" cy="262468"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="3175" cmpd="sng">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent5"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent5"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1000"/>
+                <a:t>Company</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="37" name="进程 36"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6845300" y="3251200"/>
+              <a:ext cx="141800" cy="141800"/>
+            </a:xfrm>
+            <a:prstGeom prst="flowChartProcess">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="24" name="组 23"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="7962900" y="3200400"/>
+            <a:ext cx="1003300" cy="262468"/>
+            <a:chOff x="6845300" y="3200400"/>
+            <a:chExt cx="1003300" cy="262468"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="34" name="矩形 33"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6997699" y="3200400"/>
+              <a:ext cx="850901" cy="262468"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="3175" cmpd="sng">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent5"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent5"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1000"/>
+                <a:t>Student</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="35" name="进程 34"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6845300" y="3251200"/>
+              <a:ext cx="141800" cy="141800"/>
+            </a:xfrm>
+            <a:prstGeom prst="flowChartProcess">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="25" name="组 24"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="8928100" y="3200400"/>
+            <a:ext cx="1003300" cy="262468"/>
+            <a:chOff x="6845300" y="3200400"/>
+            <a:chExt cx="1003300" cy="262468"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="32" name="矩形 31"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6997699" y="3200400"/>
+              <a:ext cx="850901" cy="262468"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="3175" cmpd="sng">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent5"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent5"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1000"/>
+                <a:t>Migrant</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="33" name="进程 32"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6845300" y="3251200"/>
+              <a:ext cx="141800" cy="141800"/>
+            </a:xfrm>
+            <a:prstGeom prst="flowChartProcess">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="26" name="组 25"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="9906000" y="3200400"/>
+            <a:ext cx="1003300" cy="262468"/>
+            <a:chOff x="6845300" y="3200400"/>
+            <a:chExt cx="1003300" cy="262468"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="30" name="矩形 29"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6997699" y="3200400"/>
+              <a:ext cx="850901" cy="262468"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="3175" cmpd="sng">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent5"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent5"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1000"/>
+                <a:t>Kiwi</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="31" name="进程 30"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6845300" y="3251200"/>
+              <a:ext cx="141800" cy="141800"/>
+            </a:xfrm>
+            <a:prstGeom prst="flowChartProcess">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="27" name="组 26"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="10604500" y="3200400"/>
+            <a:ext cx="1448394" cy="262468"/>
+            <a:chOff x="8877300" y="4114800"/>
+            <a:chExt cx="1448394" cy="262468"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="28" name="矩形 27"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9029697" y="4114800"/>
+              <a:ext cx="1295997" cy="262468"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="3175" cmpd="sng">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent5"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent5"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1000"/>
+                <a:t>Career</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-CN" sz="1000" baseline="0"/>
+                <a:t> Changer</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="29" name="进程 28"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8877300" y="4165600"/>
+              <a:ext cx="141800" cy="141800"/>
+            </a:xfrm>
+            <a:prstGeom prst="flowChartProcess">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1231899</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="矩形 37"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4038599" y="4127500"/>
+          <a:ext cx="2590800" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="3175" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>393700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="矩形 38"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2768600" y="4495800"/>
+          <a:ext cx="6743700" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="线形标注 2 (无边框) 39"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9080500" y="3683000"/>
+          <a:ext cx="2019300" cy="546100"/>
+        </a:xfrm>
+        <a:prstGeom prst="callout2">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 18750"/>
+            <a:gd name="adj2" fmla="val -8333"/>
+            <a:gd name="adj3" fmla="val 18750"/>
+            <a:gd name="adj4" fmla="val -16667"/>
+            <a:gd name="adj5" fmla="val 170640"/>
+            <a:gd name="adj6" fmla="val -39211"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>&lt;2&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>New data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> / new DB item</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="组 1"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="279400" y="254000"/>
+          <a:ext cx="11125201" cy="5918200"/>
+          <a:chOff x="279399" y="254000"/>
+          <a:chExt cx="11125201" cy="5918200"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="进程 2"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="279400" y="254000"/>
+            <a:ext cx="11125200" cy="664966"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartProcess">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent2"/>
+          </a:lnRef>
+          <a:fillRef idx="3">
+            <a:schemeClr val="accent2"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400"/>
+              <a:t>Header :</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+              <a:t> Dashboard (Common)</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="进程 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="279400" y="5706724"/>
+            <a:ext cx="11125200" cy="465476"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartProcess">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent2"/>
+          </a:lnRef>
+          <a:fillRef idx="3">
+            <a:schemeClr val="accent2"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1600"/>
+              <a:t>Footer : Contact Info. (Common) </a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1600"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="同侧圆角矩形 4"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="279400" y="1057025"/>
+            <a:ext cx="2133601" cy="398980"/>
+          </a:xfrm>
+          <a:prstGeom prst="round2SameRect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent3"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent3"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent3"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Quick Links</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="同侧圆角矩形 5"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="279400" y="2835810"/>
+            <a:ext cx="2133601" cy="398980"/>
+          </a:xfrm>
+          <a:prstGeom prst="round2SameRect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent3"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent3"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent3"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>XXX Links</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="矩形 6"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="279399" y="1472629"/>
+            <a:ext cx="2133601" cy="1263436"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent3"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent3"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="矩形 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="279399" y="3251414"/>
+            <a:ext cx="2133601" cy="2323886"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent3"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent3"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>431800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="矩形 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2768600" y="3162300"/>
+          <a:ext cx="6743700" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="线形标注 2 (无边框) 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9080500" y="2311400"/>
+          <a:ext cx="2019300" cy="546100"/>
+        </a:xfrm>
+        <a:prstGeom prst="callout2">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 18750"/>
+            <a:gd name="adj2" fmla="val -8333"/>
+            <a:gd name="adj3" fmla="val 18750"/>
+            <a:gd name="adj4" fmla="val -16667"/>
+            <a:gd name="adj5" fmla="val 170640"/>
+            <a:gd name="adj6" fmla="val -39211"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>&lt;1&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>New data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> / new DB item</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1231899</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>618066</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="可选流程 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4038599" y="5054600"/>
+          <a:ext cx="859367" cy="241300"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartAlternateProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="0" rIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="800"/>
+            <a:t>Submit</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1231899</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>330200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="矩形 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4038599" y="1371600"/>
+          <a:ext cx="2590800" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="3175" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Software</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Testing</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1231899</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>78317</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>332317</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="矩形 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4038599" y="1830917"/>
+          <a:ext cx="2590800" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="3175" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>SLT001</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1231899</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>86785</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>340785</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="矩形 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4038599" y="3668185"/>
+          <a:ext cx="2590800" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="3175" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>xxxxx</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1231899</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>211667</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="矩形 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4093632" y="4601633"/>
+          <a:ext cx="452968" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="3175" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>8</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1231899</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>80434</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>334434</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="16" name="组 15"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4038599" y="2290234"/>
+          <a:ext cx="2590800" cy="254000"/>
+          <a:chOff x="4038599" y="2290234"/>
+          <a:chExt cx="2590800" cy="254000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="17" name="矩形 16"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4038599" y="2290234"/>
+            <a:ext cx="2590800" cy="254000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln w="3175" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent5"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent5"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+              <a:t>Please select </a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="18" name="合并 17"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6400800" y="2349500"/>
+            <a:ext cx="180000" cy="141800"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartMerge">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1231899</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>82551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>336551</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="19" name="组 18"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4038599" y="2749551"/>
+          <a:ext cx="2590800" cy="254000"/>
+          <a:chOff x="4038599" y="2749551"/>
+          <a:chExt cx="2590800" cy="254000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="20" name="矩形 19"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4038599" y="2749551"/>
+            <a:ext cx="2590800" cy="254000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln w="3175" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent5"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent5"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+              <a:t>Please select</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="21" name="合并 20"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6400800" y="2806700"/>
+            <a:ext cx="180000" cy="141800"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartMerge">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1231899</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>64093</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>376768</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="22" name="组 21"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4038599" y="3238500"/>
+          <a:ext cx="5207594" cy="262468"/>
           <a:chOff x="6845300" y="3200400"/>
           <a:chExt cx="5207594" cy="262468"/>
         </a:xfrm>
@@ -5292,6 +5544,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>250</a:t>
+          </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -7756,8 +8012,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="292608" y="256032"/>
-          <a:ext cx="11131297" cy="5949696"/>
+          <a:off x="292100" y="254000"/>
+          <a:ext cx="11125201" cy="5918200"/>
           <a:chOff x="279399" y="254000"/>
           <a:chExt cx="11125201" cy="5918200"/>
         </a:xfrm>
@@ -8230,6 +8486,14 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Joan</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t> Smith</a:t>
+          </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -8293,6 +8557,17 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>xxxxxxxx</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>xxxxxxxx</a:t>
+          </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -8356,6 +8631,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>2</a:t>
+          </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -8382,8 +8661,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4044695" y="2362200"/>
-          <a:ext cx="2149434" cy="260944"/>
+          <a:off x="4038599" y="2349500"/>
+          <a:ext cx="2146894" cy="262468"/>
           <a:chOff x="7099299" y="2781300"/>
           <a:chExt cx="2146894" cy="262468"/>
         </a:xfrm>
@@ -8700,6 +8979,24 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>xxxxxxxxx</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>xxxxxxxxx</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>xxxxxxxxx</a:t>
+          </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -8791,8 +9088,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4044695" y="2106168"/>
-          <a:ext cx="3087624" cy="263992"/>
+          <a:off x="4038599" y="2095500"/>
+          <a:ext cx="3086100" cy="262468"/>
           <a:chOff x="6845300" y="3200400"/>
           <a:chExt cx="3086100" cy="262468"/>
         </a:xfrm>
@@ -9195,8 +9492,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4044694" y="4136136"/>
-          <a:ext cx="3008885" cy="256032"/>
+          <a:off x="4038598" y="4114800"/>
+          <a:ext cx="3007361" cy="254000"/>
           <a:chOff x="4005578" y="4274820"/>
           <a:chExt cx="3004821" cy="254000"/>
         </a:xfrm>
@@ -9394,8 +9691,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3995926" y="4412488"/>
-          <a:ext cx="3963249" cy="641604"/>
+          <a:off x="3987798" y="4386580"/>
+          <a:ext cx="3963249" cy="640080"/>
           <a:chOff x="3987798" y="4386580"/>
           <a:chExt cx="3963249" cy="640080"/>
         </a:xfrm>
@@ -10028,8 +10325,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="268223" y="256032"/>
-          <a:ext cx="11131297" cy="5955792"/>
+          <a:off x="266699" y="254000"/>
+          <a:ext cx="11125201" cy="5918200"/>
           <a:chOff x="279399" y="254000"/>
           <a:chExt cx="11125201" cy="5918200"/>
         </a:xfrm>
@@ -11090,7 +11387,7 @@
   </sheetPr>
   <dimension ref="B2:X16"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -11265,11 +11562,11 @@
         <v>6</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="U7" s="13"/>
       <c r="V7" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W7" s="15"/>
       <c r="X7" s="7"/>
@@ -11288,25 +11585,25 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="O8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="O8" s="19" t="s">
+      <c r="P8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="20" t="s">
+      <c r="Q8" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="Q8" s="20" t="s">
+      <c r="R8" s="20" t="s">
         <v>12</v>
-      </c>
-      <c r="R8" s="20" t="s">
-        <v>13</v>
       </c>
       <c r="S8" s="19">
         <v>250</v>
       </c>
       <c r="T8" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U8" s="16"/>
       <c r="V8" s="17"/>
@@ -11327,25 +11624,25 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="19" t="s">
+      <c r="P9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="P9" s="20" t="s">
+      <c r="Q9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="Q9" s="20" t="s">
+      <c r="R9" s="20" t="s">
         <v>12</v>
-      </c>
-      <c r="R9" s="20" t="s">
-        <v>13</v>
       </c>
       <c r="S9" s="19">
         <v>250</v>
       </c>
       <c r="T9" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U9" s="16"/>
       <c r="V9" s="17"/>
@@ -11366,25 +11663,25 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="O10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="19" t="s">
+      <c r="P10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="P10" s="20" t="s">
+      <c r="Q10" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="Q10" s="20" t="s">
+      <c r="R10" s="20" t="s">
         <v>12</v>
-      </c>
-      <c r="R10" s="20" t="s">
-        <v>13</v>
       </c>
       <c r="S10" s="19">
         <v>250</v>
       </c>
       <c r="T10" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U10" s="16"/>
       <c r="V10" s="17"/>
@@ -11405,25 +11702,25 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="O11" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="O11" s="19" t="s">
+      <c r="P11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="P11" s="20" t="s">
+      <c r="Q11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="Q11" s="20" t="s">
+      <c r="R11" s="20" t="s">
         <v>12</v>
-      </c>
-      <c r="R11" s="20" t="s">
-        <v>13</v>
       </c>
       <c r="S11" s="19">
         <v>250</v>
       </c>
       <c r="T11" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U11" s="16"/>
       <c r="V11" s="17"/>
@@ -11444,25 +11741,25 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="O12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="O12" s="19" t="s">
+      <c r="P12" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="P12" s="20" t="s">
+      <c r="Q12" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="Q12" s="20" t="s">
+      <c r="R12" s="20" t="s">
         <v>12</v>
-      </c>
-      <c r="R12" s="20" t="s">
-        <v>13</v>
       </c>
       <c r="S12" s="19">
         <v>250</v>
       </c>
       <c r="T12" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U12" s="16"/>
       <c r="V12" s="17"/>
@@ -11588,7 +11885,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:X22"/>
+  <dimension ref="B2:X21"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
@@ -11721,7 +12018,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -11748,7 +12045,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O7" s="22"/>
       <c r="P7" s="23"/>
@@ -11775,7 +12072,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O8" s="22"/>
       <c r="P8" s="23"/>
@@ -11802,7 +12099,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="21" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="O9" s="22"/>
       <c r="P9" s="23"/>
@@ -11829,7 +12126,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="21" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="O10" s="22"/>
       <c r="P10" s="23"/>
@@ -11856,7 +12153,7 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="21" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="O11" s="22"/>
       <c r="P11" s="23"/>
@@ -11910,7 +12207,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O13" s="22"/>
       <c r="P13" s="23"/>
@@ -11923,7 +12220,7 @@
       <c r="W13" s="24"/>
       <c r="X13" s="7"/>
     </row>
-    <row r="14" spans="2:24">
+    <row r="14" spans="2:24" ht="36" customHeight="1">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -11936,16 +12233,18 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
+      <c r="N14" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="O14" s="22"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
       <c r="X14" s="7"/>
     </row>
     <row r="15" spans="2:24">
@@ -12098,55 +12397,30 @@
       <c r="W20" s="6"/>
       <c r="X20" s="7"/>
     </row>
-    <row r="21" spans="2:24">
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6"/>
-      <c r="W21" s="6"/>
-      <c r="X21" s="7"/>
-    </row>
-    <row r="22" spans="2:24">
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
-      <c r="W22" s="10"/>
-      <c r="X22" s="11"/>
+    <row r="21" spans="2:24" ht="10" customHeight="1">
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -12300,7 +12574,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -12327,7 +12601,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O7" s="22"/>
       <c r="P7" s="23"/>
@@ -12354,7 +12628,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O8" s="22"/>
       <c r="P8" s="23"/>
@@ -12381,7 +12655,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O9" s="22"/>
       <c r="P9" s="23"/>
@@ -12408,7 +12682,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O10" s="22"/>
       <c r="P10" s="23"/>
@@ -12435,7 +12709,7 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="21" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="O11" s="22"/>
       <c r="P11" s="23"/>
@@ -12489,7 +12763,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O13" s="22"/>
       <c r="P13" s="23"/>
@@ -12516,7 +12790,7 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O14" s="22"/>
       <c r="P14" s="23"/>
@@ -12856,7 +13130,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -12883,7 +13157,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O7" s="22"/>
       <c r="P7" s="23"/>
@@ -12910,7 +13184,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="O8" s="22"/>
       <c r="P8" s="23"/>
@@ -12937,7 +13211,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="21" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="O9" s="22"/>
       <c r="P9" s="23"/>
@@ -12989,7 +13263,7 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O11" s="22"/>
       <c r="P11" s="23"/>
@@ -13016,7 +13290,7 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O12" s="22"/>
       <c r="P12" s="23"/>
@@ -13043,7 +13317,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O13" s="22"/>
       <c r="P13" s="23"/>
@@ -13095,7 +13369,7 @@
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="O15" s="22"/>
       <c r="P15" s="23"/>
@@ -13435,7 +13709,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -13462,7 +13736,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O7" s="22"/>
       <c r="P7" s="23"/>
@@ -13489,7 +13763,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="O8" s="22"/>
       <c r="P8" s="23"/>
@@ -13516,7 +13790,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="21" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="O9" s="22"/>
       <c r="P9" s="23"/>
@@ -13568,7 +13842,7 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O11" s="22"/>
       <c r="P11" s="23"/>
@@ -13595,7 +13869,7 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O12" s="22"/>
       <c r="P12" s="23"/>
@@ -13622,7 +13896,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O13" s="22"/>
       <c r="P13" s="23"/>
@@ -13674,7 +13948,7 @@
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="O15" s="22"/>
       <c r="P15" s="23"/>
@@ -13883,7 +14157,7 @@
   </sheetPr>
   <dimension ref="B2:V16"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -14004,7 +14278,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -14029,24 +14303,24 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="R7" s="32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="S7" s="33"/>
       <c r="T7" s="13"/>
       <c r="U7" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V7" s="7"/>
     </row>
@@ -14064,22 +14338,22 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="O8" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q8" s="20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="R8" s="30" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="S8" s="31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T8" s="16"/>
       <c r="U8" s="18"/>
@@ -14099,22 +14373,22 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="R9" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="O9" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="P9" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q9" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="R9" s="30" t="s">
-        <v>41</v>
-      </c>
       <c r="S9" s="31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T9" s="16"/>
       <c r="U9" s="18"/>
@@ -14134,22 +14408,22 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="P10" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q10" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="O10" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="P10" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q10" s="20" t="s">
-        <v>43</v>
-      </c>
       <c r="R10" s="30" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="S10" s="31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T10" s="16"/>
       <c r="U10" s="18"/>
@@ -14169,22 +14443,22 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="O11" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="P11" s="20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q11" s="20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="R11" s="30" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="S11" s="31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T11" s="16"/>
       <c r="U11" s="18"/>

</xml_diff>